<commit_message>
Adds cutout for LED strips in lower airframe.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ppak1\GitHub\Comet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012007BB-B90C-4CAB-ADAF-3ADA27CE62C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{012007BB-B90C-4CAB-ADAF-3ADA27CE62C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CFD5F05-27EB-405B-8210-406E92C5CF3A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{590520B0-EA7F-4D81-A8E7-19BCBCBD4262}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="16">
   <si>
     <t>Item</t>
   </si>
@@ -60,6 +58,24 @@
   </si>
   <si>
     <t>38 mm 1080 Motor Casing</t>
+  </si>
+  <si>
+    <t>38mm Forward Closure Plugged Threaded (apogeerockets.com)</t>
+  </si>
+  <si>
+    <t>38 mm Forward Closure Plugged Threaded</t>
+  </si>
+  <si>
+    <t>38mm Aft Closure (apogeerockets.com)</t>
+  </si>
+  <si>
+    <t>38 mm Aft Closure</t>
+  </si>
+  <si>
+    <t>Aero Pack 38mm Retainer (RA38PH) – Aeropack</t>
+  </si>
+  <si>
+    <t>38 mm Motor Retainer</t>
   </si>
 </sst>
 </file>
@@ -107,10 +123,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,19 +465,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE784CDC-BC62-4760-BA20-6C5EA9598184}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="4" max="4" width="115.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.2421875" customWidth="1"/>
+    <col min="2" max="2" width="10.0859375" customWidth="1"/>
+    <col min="3" max="3" width="10.4921875" customWidth="1"/>
+    <col min="4" max="4" width="115.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,7 +493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -486,7 +507,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -498,12 +519,57 @@
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>58.88</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>51.1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="https://aerotech-rocketry.com/products/aerotech-38mm-motor-mount-tube-13824" xr:uid="{CAE7EF40-5335-4327-A195-7878D2B16B2C}"/>
     <hyperlink ref="D3" r:id="rId2" display="https://www.apogeerockets.com/Rocket_Motors/Rouse-Tech_Casings/38mm_Casings/RMS-38_1080_Casing" xr:uid="{41C21067-A867-45F4-A2B8-DCBB0CF40F74}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{0BF6D93C-BB3A-4BD1-B039-511D3CAB7B53}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{C32C0BE3-E9F7-49D3-8A2C-A92EDEC49AE2}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{92153C9F-A8D9-441A-B8C4-34FB133A8397}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adds updated BOM and solidworks files.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ppak1\GitHub\Comet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{012007BB-B90C-4CAB-ADAF-3ADA27CE62C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CFD5F05-27EB-405B-8210-406E92C5CF3A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB94C629-DCA7-4FAE-AADB-2CEF5210F50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{590520B0-EA7F-4D81-A8E7-19BCBCBD4262}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Item</t>
   </si>
@@ -72,10 +72,52 @@
     <t>38 mm Aft Closure</t>
   </si>
   <si>
-    <t>Aero Pack 38mm Retainer (RA38PH) – Aeropack</t>
-  </si>
-  <si>
     <t>38 mm Motor Retainer</t>
+  </si>
+  <si>
+    <t>Heat-Set Inserts for Plastic, Brass, M3 x 0.5 mm, 5.7 mm Installed Length | McMaster-Carr</t>
+  </si>
+  <si>
+    <t>M3 x 0.5mm x 5.7 mm Heat Inserts</t>
+  </si>
+  <si>
+    <t>StratoLoggerCF</t>
+  </si>
+  <si>
+    <t>SLCF (perfectflite.com)</t>
+  </si>
+  <si>
+    <t>Alloy Steel Socket Head Screw, Black-Oxide, M3 x 0.5 mm Thread, 8 mm Long | McMaster-Carr</t>
+  </si>
+  <si>
+    <t>M3 x 0.5mm x 8 Screw</t>
+  </si>
+  <si>
+    <t>AeroTech J825R-14A RMS-38/1080 Reload Kit (1 Pack) - 108214 – AeroTech/Quest Division, RCS Rocket Motor Components, Inc (aerotech-rocketry.com)</t>
+  </si>
+  <si>
+    <t>J825R-14A-RMS-38/1080 Motor Reload</t>
+  </si>
+  <si>
+    <t>AeroTech RMS-38 38mm Plugged Threaded Forward Closure - 38FCPT – AeroTech/Quest Division, RCS Rocket Motor Components, Inc (aerotech-rocketry.com)</t>
+  </si>
+  <si>
+    <t>Alternate Link</t>
+  </si>
+  <si>
+    <t>AeroTech RMS-38 38mm 1080 N-Sec Aluminum Motor Case - 3810CA – AeroTech/Quest Division, RCS Rocket Motor Components, Inc (aerotech-rocketry.com)</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Bill of Materials</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>RA38P, Retainer Assembly, 38mm, P – Aeropack</t>
   </si>
 </sst>
 </file>
@@ -85,7 +127,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +139,22 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,13 +181,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -465,112 +525,230 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE784CDC-BC62-4760-BA20-6C5EA9598184}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.2421875" customWidth="1"/>
-    <col min="2" max="2" width="10.0859375" customWidth="1"/>
-    <col min="3" max="3" width="10.4921875" customWidth="1"/>
-    <col min="4" max="4" width="115.5546875" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="138.140625" customWidth="1"/>
+    <col min="5" max="5" width="91.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>131.44</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>116.99</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>58.88</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>52.99</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
         <v>51.1</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>115.99</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f>SUM(C5:C10)</f>
+        <v>364.07</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2">
+        <v>14.25</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>12</v>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>69.95</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://aerotech-rocketry.com/products/aerotech-38mm-motor-mount-tube-13824" xr:uid="{CAE7EF40-5335-4327-A195-7878D2B16B2C}"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://www.apogeerockets.com/Rocket_Motors/Rouse-Tech_Casings/38mm_Casings/RMS-38_1080_Casing" xr:uid="{41C21067-A867-45F4-A2B8-DCBB0CF40F74}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{0BF6D93C-BB3A-4BD1-B039-511D3CAB7B53}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{C32C0BE3-E9F7-49D3-8A2C-A92EDEC49AE2}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{92153C9F-A8D9-441A-B8C4-34FB133A8397}"/>
+    <hyperlink ref="D5" r:id="rId1" display="https://aerotech-rocketry.com/products/aerotech-38mm-motor-mount-tube-13824" xr:uid="{CAE7EF40-5335-4327-A195-7878D2B16B2C}"/>
+    <hyperlink ref="E6" r:id="rId2" display="https://www.apogeerockets.com/Rocket_Motors/Rouse-Tech_Casings/38mm_Casings/RMS-38_1080_Casing" xr:uid="{41C21067-A867-45F4-A2B8-DCBB0CF40F74}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{0BF6D93C-BB3A-4BD1-B039-511D3CAB7B53}"/>
+    <hyperlink ref="D8" r:id="rId4" xr:uid="{C32C0BE3-E9F7-49D3-8A2C-A92EDEC49AE2}"/>
+    <hyperlink ref="D15" r:id="rId5" xr:uid="{7168EB3F-6AFF-4E01-98DA-D987EF59C9CD}"/>
+    <hyperlink ref="D16" r:id="rId6" display="http://www.perfectflite.com/SLCF.html" xr:uid="{2EEB982D-1FC6-4F5E-9F92-6264468B369B}"/>
+    <hyperlink ref="D17" r:id="rId7" display="https://www.mcmaster.com/91290A113/" xr:uid="{0C89F8BA-EB60-44B3-B1EF-D40D5204147C}"/>
+    <hyperlink ref="D10" r:id="rId8" display="https://aerotech-rocketry.com/products/product_444c59d0-ab1d-ca27-ac40-ba1f874c7d20?_pos=1&amp;_sid=caee829c1&amp;_ss=r" xr:uid="{9B3D8799-2333-4EC4-8BE2-C85F97AF9722}"/>
+    <hyperlink ref="D7" r:id="rId9" display="https://aerotech-rocketry.com/products/product_23e4991d-c29e-ffc3-c08d-7856e49c1dc1?_pos=1&amp;_sid=b28b09aa8&amp;_ss=r" xr:uid="{202220BF-0CD8-4EF5-8717-DE1E94EFC8ED}"/>
+    <hyperlink ref="D6" r:id="rId10" display="https://aerotech-rocketry.com/products/product_62400dc5-2f70-214e-bb09-683e5eac178d?_pos=1&amp;_sid=7ae086bac&amp;_ss=r" xr:uid="{DEB1FC76-DAC5-4A3A-B639-06C8F00A7F16}"/>
+    <hyperlink ref="D9" r:id="rId11" display="https://aeropack.net/products/ra38p-retainer-assembly-38mm-p?pr_prod_strat=e5_desc&amp;pr_rec_id=fdb4b8d76&amp;pr_rec_pid=8459345428770&amp;pr_ref_pid=8459346870562&amp;pr_seq=uniform" xr:uid="{16F82A2C-C9E7-4F41-834C-E751D0C4F495}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>